<commit_message>
water volume to withdraw
</commit_message>
<xml_diff>
--- a/crop_parameters.xlsx
+++ b/crop_parameters.xlsx
@@ -21,19 +21,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Fruits</t>
-  </si>
-  <si>
-    <t>Vegetables</t>
-  </si>
-  <si>
-    <t>Maize_Cassava_Beans</t>
-  </si>
-  <si>
     <t>irrigation_volume</t>
   </si>
   <si>
     <t>revenue</t>
+  </si>
+  <si>
+    <t>maize_cassava_beans</t>
+  </si>
+  <si>
+    <t>vegetables</t>
+  </si>
+  <si>
+    <t>fruits</t>
   </si>
 </sst>
 </file>
@@ -354,7 +354,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -366,10 +366,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -377,7 +377,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -391,7 +391,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>4</v>

</xml_diff>

<commit_message>
update parameters for Canal do Sertão. update plots to deal with multiple model runs (and therefore calculate uncertainty)
</commit_message>
<xml_diff>
--- a/crop_parameters.xlsx
+++ b/crop_parameters.xlsx
@@ -1,28 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_5CAE12107CB2F49D9719FC86D39FA03B3A4EDBBA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BC25A38-9B41-4D9A-9041-B6736C516417}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>irrigation_volume</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>revenue</t>
   </si>
@@ -34,12 +43,18 @@
   </si>
   <si>
     <t>fruits</t>
+  </si>
+  <si>
+    <t>share</t>
+  </si>
+  <si>
+    <t>irrigation_requirement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -69,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -86,6 +102,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -350,57 +370,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>754.3</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>818.4</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>768.7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
+        <v>29394</v>
+      </c>
+      <c r="C3" s="1">
+        <v>105427.35042735044</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5084.0157954935976</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
+      <c r="B4">
+        <v>0.54008438818565396</v>
+      </c>
+      <c r="C4">
+        <v>0.21518987341772153</v>
+      </c>
+      <c r="D4">
+        <v>0.24472573839662448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>